<commit_message>
Remove completed items and update high priorities in competitor analysis
REMOVED (Completed):
- Sponsor Matching AI
- Verification System
- Dashboard Savings Display

NEW HIGH PRIORITIES (5 items):
1. Event Collaboration/Co-hosting - Multi-host events, revenue splits, tour tracking
2. Promoter Referral System - Role-based affiliate program with tracking links
3. Landing Page Overhaul - 2-tier pricing, ROI focus, hide competitor comparison
4. Venue Partnership System - Venue lock-in strategy for market domination
5. Revenue Stream Documentation - Monetization strategy for free events

Focus: Venue partnerships as competitive moat, "pay when paid" psychology
</commit_message>
<xml_diff>
--- a/SponsorSynq_Competitor_Comparison.xlsx
+++ b/SponsorSynq_Competitor_Comparison.xlsx
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -68,12 +68,8 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <i val="1"/>
-      <color rgb="0070AD47"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill/>
     </fill>
@@ -124,12 +120,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E2EFDA"/>
-        <bgColor rgb="00E2EFDA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00FF9900"/>
         <bgColor rgb="00FF9900"/>
       </patternFill>
@@ -159,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -200,16 +190,13 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1904,7 +1891,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1991,100 +1978,12 @@
       </c>
     </row>
     <row r="10" ht="120" customHeight="1">
-      <c r="A10" s="14" t="inlineStr">
-        <is>
-          <t>✓ Sponsor Matching</t>
-        </is>
-      </c>
-      <c r="B10" s="14" t="inlineStr">
-        <is>
-          <t>Build excellent AI matching algorithm</t>
-        </is>
-      </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>Our 12% commission must feel justified by quality matches</t>
-        </is>
-      </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="120" customHeight="1">
-      <c r="A11" s="14" t="inlineStr">
-        <is>
-          <t>✓ Verification System</t>
-        </is>
-      </c>
-      <c r="B11" s="14" t="inlineStr">
-        <is>
-          <t>Robust photo upload + attendance tracking</t>
-        </is>
-      </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>Sponsors need proof their money worked</t>
-        </is>
-      </c>
-      <c r="D11" s="14" t="inlineStr">
-        <is>
-          <t>COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="120" customHeight="1">
-      <c r="A12" s="14" t="inlineStr">
-        <is>
-          <t>✓ Dashboard Savings Display</t>
-        </is>
-      </c>
-      <c r="B12" s="14" t="inlineStr">
-        <is>
-          <t>Show subscribers monthly savings vs 5%</t>
-        </is>
-      </c>
-      <c r="C12" s="14" t="inlineStr">
-        <is>
-          <t>Psychological win every month</t>
-        </is>
-      </c>
-      <c r="D12" s="14" t="inlineStr">
-        <is>
-          <t>COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="120" customHeight="1">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>Ambassador Visibility</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>Prominently feature program in UI</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>Users won't discover it unless we surface it</t>
-        </is>
-      </c>
-      <c r="D13" s="3" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="120" customHeight="1">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>Event Collaboration/Co-hosting</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>Multi-host event collaboration system:
 • Primary &amp; secondary event hosts
@@ -2096,24 +1995,24 @@
 • Track all events under one tour umbrella</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>Game-changer for large-scale events and tours. Creates network effects - hosts bring other hosts. Differentiates us from all competitors who only support single-host events.</t>
         </is>
       </c>
-      <c r="D14" s="3" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="120" customHeight="1">
-      <c r="A15" s="3" t="inlineStr">
+    <row r="11" ht="120" customHeight="1">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>Promoter Referral System</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>Role-based promoter program:
 • Event hosts assign 'promoter' roles
@@ -2124,24 +2023,24 @@
 • Promoters share on Instagram/TikTok stories</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Viral growth engine. Turns every event into distributed sales team. Promoters are incentivized to drive ticket sales. Event hosts get free marketing.</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="120" customHeight="1">
-      <c r="A16" s="3" t="inlineStr">
+    <row r="12" ht="120" customHeight="1">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>Landing Page Overhaul</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>PRICING: Only 2 tiers:
 • Free: Unlimited events, basic features
@@ -2158,24 +2057,24 @@
 • Prevent competitors from copying our strategy</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>Simplicity converts better. People don't want subscriptions - they want to 'pay when they get paid' or see clear ROI. Hiding competitor intel protects our competitive advantage.</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="120" customHeight="1">
-      <c r="A17" s="3" t="inlineStr">
+    <row r="13" ht="120" customHeight="1">
+      <c r="A13" s="3" t="inlineStr">
         <is>
           <t>Venue Partnership System</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
         <is>
           <t>Venue integration features:
 • Venues can create accounts
@@ -2191,24 +2090,24 @@
 • Market domination through venue partnerships</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>This is the ULTIMATE competitive moat. If venues require SponsorSynq, event hosts have no choice. We stop competing on features and own the distribution channel. Venue adoption = market domination.</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr">
+      <c r="D13" s="3" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="120" customHeight="1">
-      <c r="A18" s="3" t="inlineStr">
+    <row r="14" ht="120" customHeight="1">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>Revenue Stream Documentation</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B14" s="3" t="inlineStr">
         <is>
           <t>Comprehensive revenue analysis:
 • Document ALL current revenue streams
@@ -2220,204 +2119,204 @@
 • Alternative revenue from free event hosts?</t>
         </is>
       </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Need clarity on business model edge cases. Free events still have value (brand awareness, sponsor discovery) but need strategy to ensure sustainable revenue. Must balance growth with monetization.</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="5" customHeight="1"/>
+    <row r="16">
+      <c r="A16" s="14" t="inlineStr">
+        <is>
+          <t>MEDIUM PRIORITY</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="15" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="B17" s="15" t="inlineStr">
+        <is>
+          <t>What To Build/Do</t>
+        </is>
+      </c>
+      <c r="C17" s="15" t="inlineStr">
+        <is>
+          <t>Why It Matters</t>
+        </is>
+      </c>
+      <c r="D17" s="15" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Performance Tracking</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Track Boost &amp; Featured Placement results</t>
+        </is>
+      </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>Need clarity on business model edge cases. Free events still have value (brand awareness, sponsor discovery) but need strategy to ensure sustainable revenue. Must balance growth with monetization.</t>
+          <t>Need data to prove these upgrades work</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="5" customHeight="1"/>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Instant Payout Cap</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Implement 1.5% with $15 max</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Makes instant payout attractive for large payouts</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
     <row r="20">
-      <c r="A20" s="15" t="inlineStr">
-        <is>
-          <t>MEDIUM PRIORITY</t>
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Annual Subscription</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Offer $190/year option</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Locks in committed hosts, improves predictability</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="16" t="inlineStr">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>Tiered Boost Options</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>$10/3d, $15/7d, $25/14d</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Flexibility for different event timelines</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="5" customHeight="1"/>
+    <row r="23">
+      <c r="A23" s="16" t="inlineStr">
+        <is>
+          <t>LOW PRIORITY</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="17" t="inlineStr">
         <is>
           <t>Area</t>
         </is>
       </c>
-      <c r="B21" s="16" t="inlineStr">
+      <c r="B24" s="17" t="inlineStr">
         <is>
           <t>What To Build/Do</t>
         </is>
       </c>
-      <c r="C21" s="16" t="inlineStr">
+      <c r="C24" s="17" t="inlineStr">
         <is>
           <t>Why It Matters</t>
         </is>
       </c>
-      <c r="D21" s="16" t="inlineStr">
+      <c r="D24" s="17" t="inlineStr">
         <is>
           <t>Priority</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="3" t="inlineStr">
-        <is>
-          <t>Performance Tracking</t>
-        </is>
-      </c>
-      <c r="B22" s="3" t="inlineStr">
-        <is>
-          <t>Track Boost &amp; Featured Placement results</t>
-        </is>
-      </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>Need data to prove these upgrades work</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t>Instant Payout Cap</t>
-        </is>
-      </c>
-      <c r="B23" s="3" t="inlineStr">
-        <is>
-          <t>Implement 1.5% with $15 max</t>
-        </is>
-      </c>
-      <c r="C23" s="3" t="inlineStr">
-        <is>
-          <t>Makes instant payout attractive for large payouts</t>
-        </is>
-      </c>
-      <c r="D23" s="3" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="inlineStr">
-        <is>
-          <t>Annual Subscription</t>
-        </is>
-      </c>
-      <c r="B24" s="3" t="inlineStr">
-        <is>
-          <t>Offer $190/year option</t>
-        </is>
-      </c>
-      <c r="C24" s="3" t="inlineStr">
-        <is>
-          <t>Locks in committed hosts, improves predictability</t>
-        </is>
-      </c>
-      <c r="D24" s="3" t="inlineStr">
-        <is>
-          <t>MEDIUM</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Tiered Boost Options</t>
+          <t>Enterprise Compliance</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>$10/3d, $15/7d, $25/14d</t>
+          <t>Approval workflows, audit trails, SIS integration</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>Flexibility for different event timelines</t>
+          <t>Required for university sales</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>MEDIUM</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="5" customHeight="1"/>
-    <row r="27">
-      <c r="A27" s="17" t="inlineStr">
-        <is>
-          <t>LOW PRIORITY</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="18" t="inlineStr">
-        <is>
-          <t>Area</t>
-        </is>
-      </c>
-      <c r="B28" s="18" t="inlineStr">
-        <is>
-          <t>What To Build/Do</t>
-        </is>
-      </c>
-      <c r="C28" s="18" t="inlineStr">
-        <is>
-          <t>Why It Matters</t>
-        </is>
-      </c>
-      <c r="D28" s="18" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="3" t="inlineStr">
-        <is>
-          <t>Enterprise Compliance</t>
-        </is>
-      </c>
-      <c r="B29" s="3" t="inlineStr">
-        <is>
-          <t>Approval workflows, audit trails, SIS integration</t>
-        </is>
-      </c>
-      <c r="C29" s="3" t="inlineStr">
-        <is>
-          <t>Required for university sales</t>
-        </is>
-      </c>
-      <c r="D29" s="3" t="inlineStr">
-        <is>
           <t>LOW</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="3" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
         <is>
           <t>Leaderboards</t>
         </is>
       </c>
-      <c r="B30" s="3" t="inlineStr">
+      <c r="B26" s="3" t="inlineStr">
         <is>
           <t>Show top ambassadors</t>
         </is>
       </c>
-      <c r="C30" s="3" t="inlineStr">
+      <c r="C26" s="3" t="inlineStr">
         <is>
           <t>Creates competition, shows what's possible</t>
         </is>
       </c>
-      <c r="D30" s="3" t="inlineStr">
+      <c r="D26" s="3" t="inlineStr">
         <is>
           <t>LOW</t>
         </is>
@@ -2427,13 +2326,13 @@
   <mergeCells count="9">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A23:D23"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A16:D16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>